<commit_message>
truncated log pearson III distribution in model to [0.01, 0.999] added a few unit tests at each level of lp3 implementation.
Former-commit-id: 270b1f30f0ef6604647b0c311e36a369164b2060
</commit_message>
<xml_diff>
--- a/FunctionsTests/ExcelTesting/ExcelData/CoordinatesFunctionsConstants.xlsx
+++ b/FunctionsTests/ExcelTesting/ExcelData/CoordinatesFunctionsConstants.xlsx
@@ -6639,7 +6639,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H7" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -6693,7 +6693,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H12" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -6747,7 +6747,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H17" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -6801,7 +6801,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H22" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -6954,7 +6954,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H7" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="I7" s="82" t="s">
         <x:v>13</x:v>
@@ -7035,7 +7035,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H12" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="I12" s="82" t="s">
         <x:v>13</x:v>
@@ -7116,7 +7116,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H17" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="I17" s="82" t="s">
         <x:v>13</x:v>
@@ -7197,7 +7197,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H22" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="I22" s="82" t="s">
         <x:v>13</x:v>
@@ -7278,7 +7278,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H27" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="I27" s="86" t="s">
         <x:v>13</x:v>
@@ -7359,7 +7359,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H32" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="I32" s="86" t="s">
         <x:v>13</x:v>
@@ -7440,7 +7440,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H37" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="I37" s="86" t="s">
         <x:v>13</x:v>
@@ -7529,7 +7529,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H42" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="I42" s="86" t="s">
         <x:v>13</x:v>
@@ -7610,7 +7610,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H47" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="I47" s="86" t="s">
         <x:v>13</x:v>
@@ -7691,7 +7691,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H52" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="I52" s="86" t="s">
         <x:v>13</x:v>
@@ -7994,7 +7994,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J7" s="37">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K7" s="37" t="s"/>
       <x:c r="L7" s="38" t="s"/>
@@ -8780,7 +8780,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="J24" s="37">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K24" s="37" t="s"/>
       <x:c r="L24" s="38" t="s"/>
@@ -9659,7 +9659,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J43" s="37">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K43" s="50" t="s"/>
       <x:c r="M43" s="32" t="s">
@@ -10259,7 +10259,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J61" s="37">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K61" s="50" t="s"/>
       <x:c r="M61" s="29" t="s">
@@ -10870,7 +10870,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J81" s="37">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K81" s="50" t="s"/>
       <x:c r="M81" s="29" t="s">
@@ -12092,7 +12092,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J121" s="37">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K121" s="50" t="s"/>
       <x:c r="M121" s="29" t="s">
@@ -12707,7 +12707,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J141" s="37">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K141" s="50" t="s"/>
       <x:c r="M141" s="29" t="s">
@@ -13321,7 +13321,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J161" s="37">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K161" s="50" t="s"/>
       <x:c r="M161" s="29" t="s">
@@ -13932,7 +13932,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J181" s="37">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K181" s="50" t="s"/>
       <x:c r="M181" s="29" t="s">
@@ -14574,7 +14574,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J201" s="37">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K201" s="50" t="s"/>
       <x:c r="M201" s="29" t="s">
@@ -15185,7 +15185,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J221" s="37">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K221" s="50" t="s"/>
       <x:c r="M221" s="29" t="s">
@@ -15796,7 +15796,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J241" s="37">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K241" s="50" t="s"/>
       <x:c r="M241" s="29" t="s">
@@ -16407,7 +16407,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J261" s="37">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K261" s="50" t="s"/>
       <x:c r="M261" s="29" t="s">
@@ -18803,7 +18803,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H7" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -18863,7 +18863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H12" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -18932,7 +18932,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H17" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -19001,7 +19001,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H22" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="I22" s="14" t="s">
         <x:v>29</x:v>
@@ -19241,7 +19241,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H7" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -19310,7 +19310,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H12" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -19371,7 +19371,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H17" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -19440,7 +19440,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H22" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -19664,7 +19664,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H7" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -19733,7 +19733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H12" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -19802,7 +19802,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H17" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -19871,7 +19871,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H22" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -19940,7 +19940,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H27" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -20009,7 +20009,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H32" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -20078,7 +20078,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H37" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -20147,7 +20147,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H42" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -20216,7 +20216,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H47" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -20285,7 +20285,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H52" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -20357,7 +20357,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H57" s="53">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -20426,7 +20426,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H62" s="53">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -20575,7 +20575,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H7" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -20644,7 +20644,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H12" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -20713,7 +20713,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H17" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -20782,7 +20782,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H22" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -20851,7 +20851,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H27" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -20920,7 +20920,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H32" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -20989,7 +20989,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H37" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:16" s="0" customFormat="1" x14ac:dyDescent="0.25">
@@ -21076,7 +21076,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H42" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -21145,7 +21145,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H47" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -21214,7 +21214,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H52" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:16" x14ac:dyDescent="0.25">
@@ -21356,7 +21356,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H7" s="54">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="I7" s="0" t="s"/>
     </x:row>
@@ -21446,7 +21446,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H12" s="54">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="I12" s="0" t="s"/>
     </x:row>
@@ -21528,7 +21528,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H17" s="54">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="I17" s="0" t="s"/>
       <x:c r="J17" s="0" t="s"/>
@@ -21608,7 +21608,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H22" s="54">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="I22" s="0" t="s"/>
     </x:row>
@@ -21690,7 +21690,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H27" s="53">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="I27" s="0" t="s"/>
     </x:row>
@@ -21772,7 +21772,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H32" s="53">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="I32" s="0" t="s"/>
     </x:row>
@@ -21854,7 +21854,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H37" s="53">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="I37" s="0" t="s"/>
     </x:row>
@@ -21936,7 +21936,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H42" s="53">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -22017,7 +22017,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H47" s="53">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="I47" s="0" t="s"/>
     </x:row>
@@ -22099,7 +22099,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H52" s="53">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="I52" s="0" t="s"/>
     </x:row>
@@ -23727,7 +23727,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I7" s="37">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="J7" s="38" t="s"/>
       <x:c r="K7" s="34" t="n">
@@ -24472,7 +24472,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I24" s="37">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="J24" s="38" t="s"/>
       <x:c r="K24" s="32" t="s">
@@ -25302,7 +25302,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I43" s="50">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K43" s="32" t="s">
         <x:v>110</x:v>
@@ -25855,7 +25855,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I61" s="50">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K61" s="29" t="s">
         <x:v>108</x:v>
@@ -26415,7 +26415,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I81" s="50">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K81" s="29" t="s">
         <x:v>108</x:v>
@@ -27536,7 +27536,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I121" s="50">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K121" s="29" t="s">
         <x:v>108</x:v>
@@ -28100,7 +28100,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I141" s="50">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K141" s="29" t="s">
         <x:v>108</x:v>
@@ -28663,7 +28663,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I161" s="50">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K161" s="29" t="s">
         <x:v>108</x:v>
@@ -29223,7 +29223,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I181" s="50">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K181" s="29" t="s">
         <x:v>108</x:v>
@@ -29785,7 +29785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I201" s="50">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K201" s="29" t="s">
         <x:v>108</x:v>
@@ -30345,7 +30345,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I221" s="50">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K221" s="29" t="s">
         <x:v>108</x:v>
@@ -30905,7 +30905,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I241" s="50">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K241" s="29" t="s">
         <x:v>108</x:v>
@@ -31465,7 +31465,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I261" s="50">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="K261" s="29" t="s">
         <x:v>108</x:v>
@@ -32007,7 +32007,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="I280" s="53">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="281" spans="1:45" x14ac:dyDescent="0.25">
@@ -32695,7 +32695,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H7" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:10" s="0" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32764,7 +32764,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H12" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:10" s="0" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32833,7 +32833,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H17" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:10" s="0" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32902,7 +32902,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H22" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:10" s="0" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32971,7 +32971,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H27" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:10" s="0" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33040,7 +33040,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H32" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:10" s="0" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33109,7 +33109,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H37" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:10" s="0" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33178,7 +33178,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H42" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:10" s="0" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33247,7 +33247,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H47" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:10" s="0" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33328,7 +33328,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H52" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:10" s="0" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33470,7 +33470,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H7" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -33539,7 +33539,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H12" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
       <x:c r="I12" s="0" t="s"/>
       <x:c r="J12" s="0" t="s"/>
@@ -33612,7 +33612,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H17" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -33681,7 +33681,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H22" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -33750,7 +33750,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H27" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -33819,7 +33819,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H32" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -33888,7 +33888,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H37" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:14" s="0" customFormat="1" x14ac:dyDescent="0.25">
@@ -33957,7 +33957,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H42" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:14" s="0" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -34042,7 +34042,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H47" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:14" s="0" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -34111,7 +34111,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H52" s="48">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:14" s="0" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -34180,7 +34180,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H57" s="52">
-        <x:v>43964.5375</x:v>
+        <x:v>44078.8104166667</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Created a special project for calculating LPIII from old statistics library made a fix to regularized Gamma function to fix an issue that arises in cases with negative skew.
Former-commit-id: 996b09a46fd9b748d55d2dc604bf2cae96bbdd32
</commit_message>
<xml_diff>
--- a/FunctionsTests/ExcelTesting/ExcelData/CoordinatesFunctionsConstants.xlsx
+++ b/FunctionsTests/ExcelTesting/ExcelData/CoordinatesFunctionsConstants.xlsx
@@ -6639,7 +6639,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H7" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -6693,7 +6693,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H12" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -6747,7 +6747,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H17" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -6801,7 +6801,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H22" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -6954,7 +6954,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H7" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="I7" s="82" t="s">
         <x:v>13</x:v>
@@ -7035,7 +7035,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H12" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="I12" s="82" t="s">
         <x:v>13</x:v>
@@ -7116,7 +7116,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H17" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="I17" s="82" t="s">
         <x:v>13</x:v>
@@ -7197,7 +7197,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H22" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="I22" s="82" t="s">
         <x:v>13</x:v>
@@ -7278,7 +7278,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H27" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="I27" s="86" t="s">
         <x:v>13</x:v>
@@ -7359,7 +7359,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H32" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="I32" s="86" t="s">
         <x:v>13</x:v>
@@ -7440,7 +7440,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H37" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="I37" s="86" t="s">
         <x:v>13</x:v>
@@ -7529,7 +7529,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H42" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="I42" s="86" t="s">
         <x:v>13</x:v>
@@ -7610,7 +7610,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H47" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="I47" s="86" t="s">
         <x:v>13</x:v>
@@ -7691,7 +7691,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H52" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="I52" s="86" t="s">
         <x:v>13</x:v>
@@ -7994,7 +7994,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J7" s="37">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K7" s="37" t="s"/>
       <x:c r="L7" s="38" t="s"/>
@@ -8780,7 +8780,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="J24" s="37">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K24" s="37" t="s"/>
       <x:c r="L24" s="38" t="s"/>
@@ -9659,7 +9659,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J43" s="37">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K43" s="50" t="s"/>
       <x:c r="M43" s="32" t="s">
@@ -10259,7 +10259,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J61" s="37">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K61" s="50" t="s"/>
       <x:c r="M61" s="29" t="s">
@@ -10870,7 +10870,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J81" s="37">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K81" s="50" t="s"/>
       <x:c r="M81" s="29" t="s">
@@ -12092,7 +12092,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J121" s="37">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K121" s="50" t="s"/>
       <x:c r="M121" s="29" t="s">
@@ -12707,7 +12707,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J141" s="37">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K141" s="50" t="s"/>
       <x:c r="M141" s="29" t="s">
@@ -13321,7 +13321,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J161" s="37">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K161" s="50" t="s"/>
       <x:c r="M161" s="29" t="s">
@@ -13932,7 +13932,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J181" s="37">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K181" s="50" t="s"/>
       <x:c r="M181" s="29" t="s">
@@ -14574,7 +14574,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J201" s="37">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K201" s="50" t="s"/>
       <x:c r="M201" s="29" t="s">
@@ -15185,7 +15185,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J221" s="37">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K221" s="50" t="s"/>
       <x:c r="M221" s="29" t="s">
@@ -15796,7 +15796,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J241" s="37">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K241" s="50" t="s"/>
       <x:c r="M241" s="29" t="s">
@@ -16407,7 +16407,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="J261" s="37">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K261" s="50" t="s"/>
       <x:c r="M261" s="29" t="s">
@@ -18803,7 +18803,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H7" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9708333333</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -18863,7 +18863,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H12" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9708333333</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -18932,7 +18932,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H17" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9708333333</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -19001,7 +19001,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H22" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9708333333</x:v>
       </x:c>
       <x:c r="I22" s="14" t="s">
         <x:v>29</x:v>
@@ -19241,7 +19241,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H7" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -19310,7 +19310,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H12" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -19371,7 +19371,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H17" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -19440,7 +19440,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H22" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -19664,7 +19664,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H7" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9708333333</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -19733,7 +19733,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H12" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9708333333</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -19802,7 +19802,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H17" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9708333333</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -19871,7 +19871,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H22" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9708333333</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -19940,7 +19940,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H27" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9708333333</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -20009,7 +20009,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H32" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9708333333</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -20078,7 +20078,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H37" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9708333333</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -20147,7 +20147,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H42" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9708333333</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -20216,7 +20216,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H47" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9708333333</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -20285,7 +20285,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H52" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9708333333</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -20357,7 +20357,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H57" s="53">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9708333333</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -20426,7 +20426,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H62" s="53">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9708333333</x:v>
       </x:c>
     </x:row>
     <x:row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -20575,7 +20575,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H7" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9708333333</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -20644,7 +20644,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H12" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9708333333</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -20713,7 +20713,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H17" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9708333333</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -20782,7 +20782,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H22" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9708333333</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -20851,7 +20851,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H27" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9708333333</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -20920,7 +20920,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H32" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9708333333</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -20989,7 +20989,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H37" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:16" s="0" customFormat="1" x14ac:dyDescent="0.25">
@@ -21076,7 +21076,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H42" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -21145,7 +21145,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H47" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -21214,7 +21214,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H52" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:16" x14ac:dyDescent="0.25">
@@ -21356,7 +21356,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H7" s="54">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="I7" s="0" t="s"/>
     </x:row>
@@ -21446,7 +21446,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H12" s="54">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="I12" s="0" t="s"/>
     </x:row>
@@ -21528,7 +21528,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H17" s="54">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="I17" s="0" t="s"/>
       <x:c r="J17" s="0" t="s"/>
@@ -21608,7 +21608,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H22" s="54">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="I22" s="0" t="s"/>
     </x:row>
@@ -21690,7 +21690,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H27" s="53">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="I27" s="0" t="s"/>
     </x:row>
@@ -21772,7 +21772,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H32" s="53">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="I32" s="0" t="s"/>
     </x:row>
@@ -21854,7 +21854,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H37" s="53">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="I37" s="0" t="s"/>
     </x:row>
@@ -21936,7 +21936,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H42" s="53">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -22017,7 +22017,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H47" s="53">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="I47" s="0" t="s"/>
     </x:row>
@@ -22099,7 +22099,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H52" s="53">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="I52" s="0" t="s"/>
     </x:row>
@@ -23727,7 +23727,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I7" s="37">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="J7" s="38" t="s"/>
       <x:c r="K7" s="34" t="n">
@@ -24472,7 +24472,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I24" s="37">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="J24" s="38" t="s"/>
       <x:c r="K24" s="32" t="s">
@@ -25302,7 +25302,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I43" s="50">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K43" s="32" t="s">
         <x:v>110</x:v>
@@ -25855,7 +25855,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I61" s="50">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K61" s="29" t="s">
         <x:v>108</x:v>
@@ -26415,7 +26415,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I81" s="50">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K81" s="29" t="s">
         <x:v>108</x:v>
@@ -27536,7 +27536,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I121" s="50">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K121" s="29" t="s">
         <x:v>108</x:v>
@@ -28100,7 +28100,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I141" s="50">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K141" s="29" t="s">
         <x:v>108</x:v>
@@ -28663,7 +28663,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I161" s="50">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K161" s="29" t="s">
         <x:v>108</x:v>
@@ -29223,7 +29223,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I181" s="50">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K181" s="29" t="s">
         <x:v>108</x:v>
@@ -29785,7 +29785,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I201" s="50">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K201" s="29" t="s">
         <x:v>108</x:v>
@@ -30345,7 +30345,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I221" s="50">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K221" s="29" t="s">
         <x:v>108</x:v>
@@ -30905,7 +30905,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I241" s="50">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K241" s="29" t="s">
         <x:v>108</x:v>
@@ -31465,7 +31465,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="I261" s="50">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="K261" s="29" t="s">
         <x:v>108</x:v>
@@ -32007,7 +32007,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="I280" s="53">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="281" spans="1:45" x14ac:dyDescent="0.25">
@@ -32695,7 +32695,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H7" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:10" s="0" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32764,7 +32764,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H12" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:10" s="0" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32833,7 +32833,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H17" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:10" s="0" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32902,7 +32902,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H22" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:10" s="0" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -32971,7 +32971,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H27" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:10" s="0" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33040,7 +33040,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H32" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:10" s="0" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33109,7 +33109,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H37" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:10" s="0" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33178,7 +33178,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H42" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:10" s="0" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33247,7 +33247,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H47" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:10" s="0" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33328,7 +33328,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="H52" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:10" s="0" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -33470,7 +33470,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H7" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -33539,7 +33539,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H12" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
       <x:c r="I12" s="0" t="s"/>
       <x:c r="J12" s="0" t="s"/>
@@ -33612,7 +33612,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H17" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -33681,7 +33681,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H22" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -33750,7 +33750,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H27" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -33819,7 +33819,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H32" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -33888,7 +33888,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H37" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:14" s="0" customFormat="1" x14ac:dyDescent="0.25">
@@ -33957,7 +33957,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H42" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:14" s="0" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -34042,7 +34042,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H47" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:14" s="0" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -34111,7 +34111,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H52" s="48">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:14" s="0" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -34180,7 +34180,7 @@
         <x:v>39</x:v>
       </x:c>
       <x:c r="H57" s="52">
-        <x:v>44078.8104166667</x:v>
+        <x:v>44091.9715277778</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>